<commit_message>
Worked the logic for opening from a CSV sheet.
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/83030895d86a704a/Documents/Personal/Coding practice/Pizza-Ordering-Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC1048B821DD58C85ADE58E4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8B9582E7-8A84-402E-9995-57B333172E53}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_F25DC773A252ABDACC1048B821DD58C85ADE58E4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2B0F93D-4D42-462C-8F9A-B6ED1E77CC8E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32280" yWindow="1200" windowWidth="21600" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Pizza Type</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Pepperoni</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>L6A 1H6</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,9 +424,10 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -443,15 +450,17 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -483,12 +492,15 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Successfully implemented saving and loading from textfield.
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/83030895d86a704a/Documents/Personal/Coding practice/Pizza-Ordering-Bot/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{2E426F4B-4087-4B60-82A3-FC6CF8471C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="32280" yWindow="1200" windowWidth="21600" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -22,8 +28,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +66,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -106,7 +120,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -138,9 +152,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -172,6 +204,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -347,14 +397,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>